<commit_message>
updated Majuro collection data
</commit_message>
<xml_diff>
--- a/sample_shipment/Majuro-collection-records.xlsx
+++ b/sample_shipment/Majuro-collection-records.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t xml:space="preserve">beetle_id</t>
   </si>
@@ -31,10 +31,16 @@
     <t xml:space="preserve">location</t>
   </si>
   <si>
-    <t xml:space="preserve">Airport, Akia, Majuru, Republic of the Marshall Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loiemno, Ajeltavie, Majuru, Republic of the Marshall Islands</t>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airport, Akia, Majuro, Republic of the Marshall Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lojemwe Weto, Ajeltake, Majuro, Republic of the Marshall Islands</t>
   </si>
 </sst>
 </file>
@@ -50,6 +56,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,17 +142,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -158,6 +165,12 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -167,7 +180,13 @@
         <v>45193</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>7.068092</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>171.281427</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -178,7 +197,13 @@
         <v>45203</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>7.084167</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>171.133889</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -189,7 +214,13 @@
         <v>45203</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>7.084167</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>171.133889</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -200,7 +231,13 @@
         <v>45203</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7.084167</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>171.133889</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,7 +248,13 @@
         <v>45203</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>7.084167</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>171.133889</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -222,7 +265,13 @@
         <v>45203</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>7.084167</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>171.133889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>